<commit_message>
right: Add RIGHT option, like DOWN but a different direction
https://github.com/OpenDataServices/spreadsheet-forms/issues/5
</commit_message>
<xml_diff>
--- a/tests/data/cat1.xlsx
+++ b/tests/data/cat1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t xml:space="preserve">Pet</t>
   </si>
@@ -33,6 +33,39 @@
   </si>
   <si>
     <t xml:space="preserve">Miaow Miaow Purr Purr Hiss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hungry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Always</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleepy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A lot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also Right Now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Nap</t>
   </si>
   <si>
     <t xml:space="preserve">Please Place Info about toys below!</t>
@@ -63,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -97,6 +130,19 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -108,13 +154,6 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -176,7 +215,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,19 +232,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -226,10 +281,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A5:B6"/>
+  <dimension ref="A5:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -254,6 +309,58 @@
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -273,7 +380,7 @@
   </sheetPr>
   <dimension ref="A2:B32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -285,130 +392,130 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
+      <c r="A2" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
+      <c r="A3" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>7</v>
+      <c r="A6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>9</v>
+      <c r="A7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>9</v>
+      <c r="A8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>